<commit_message>
converted the choice exampel exceptions using effects
</commit_message>
<xml_diff>
--- a/benchmarks/effects/results.xlsx
+++ b/benchmarks/effects/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yahuis/Desktop/git/AlgebraicEffect/benchmark/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yahuis/Desktop/git/AlgebraicEffect/benchmarks/effects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23F634F-3681-C140-8D21-98BF916D5113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D946B7C-94BD-FD4E-9D8E-E45E617DD738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="600" windowWidth="28040" windowHeight="17440" xr2:uid="{F224C7BA-0B0B-E048-B52D-6A1651DC64AD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>McCarthy_Andrej_Bauer</t>
   </si>
@@ -108,13 +108,25 @@
   </si>
   <si>
     <t>Time(ms)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Monad </t>
+  </si>
+  <si>
+    <t>Inductive sumEff</t>
+  </si>
+  <si>
+    <t>Async Yield</t>
+  </si>
+  <si>
+    <t>Exchange State</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -129,6 +141,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFAAAAAA"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -151,20 +170,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA336E8F-A7D0-AB4A-B959-3554529D4463}">
-  <dimension ref="B2:H17"/>
+  <dimension ref="A2:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,37 +515,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>56</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -535,10 +555,10 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
@@ -546,10 +566,10 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
@@ -557,14 +577,14 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>71</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -574,10 +594,10 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="1" t="s">
         <v>4</v>
       </c>
@@ -585,10 +605,10 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="1" t="s">
         <v>5</v>
       </c>
@@ -596,14 +616,14 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>69</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -613,10 +633,10 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="1" t="s">
         <v>4</v>
       </c>
@@ -624,10 +644,10 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="1" t="s">
         <v>7</v>
       </c>
@@ -635,14 +655,14 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <v>60</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -652,10 +672,10 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
       <c r="F13" s="1" t="s">
         <v>22</v>
       </c>
@@ -663,10 +683,10 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="1" t="s">
         <v>4</v>
       </c>
@@ -674,13 +694,13 @@
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <v>193</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="3"/>
       <c r="E15" s="4" t="s">
         <v>21</v>
       </c>
@@ -691,9 +711,9 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
       <c r="E16" s="4"/>
       <c r="F16" s="1" t="s">
         <v>9</v>
@@ -701,10 +721,10 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
       <c r="E17" s="4"/>
       <c r="F17" s="1" t="s">
         <v>10</v>
@@ -712,13 +732,130 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="1">
+        <v>29</v>
+      </c>
+      <c r="D22" s="1">
+        <v>6</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="1">
+        <v>19</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1">
+        <v>20</v>
+      </c>
+      <c r="D24" s="1">
+        <v>5</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="1">
+        <v>32</v>
+      </c>
+      <c r="D25" s="1">
+        <v>7</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>83</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1">
+        <v>70</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="1">
+        <v>109</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="C6:C8"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="E6:E8"/>
@@ -728,12 +865,11 @@
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D12:D14"/>
     <mergeCell ref="D6:D8"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="C12:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added the final summary
</commit_message>
<xml_diff>
--- a/benchmarks/effects/results.xlsx
+++ b/benchmarks/effects/results.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yahuis/Desktop/git/AlgebraicEffect/benchmarks/effects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D946B7C-94BD-FD4E-9D8E-E45E617DD738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4970C29C-930C-BB42-99DA-369DE76936D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="600" windowWidth="28040" windowHeight="17440" xr2:uid="{F224C7BA-0B0B-E048-B52D-6A1651DC64AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>McCarthy_Andrej_Bauer</t>
   </si>
@@ -120,6 +120,21 @@
   </si>
   <si>
     <t>Exchange State</t>
+  </si>
+  <si>
+    <t>Forward (ms)</t>
+  </si>
+  <si>
+    <t>Entailment (ms)</t>
+  </si>
+  <si>
+    <t>AskZ3 (ms)</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Totol</t>
   </si>
 </sst>
 </file>
@@ -170,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -178,13 +193,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,7 +520,7 @@
   <dimension ref="A2:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,8 +528,9 @@
     <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
@@ -538,14 +557,14 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>56</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -555,10 +574,10 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
       <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
@@ -566,10 +585,10 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
@@ -577,14 +596,14 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>71</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -594,10 +613,10 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="1" t="s">
         <v>4</v>
       </c>
@@ -605,10 +624,10 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="1" t="s">
         <v>5</v>
       </c>
@@ -616,14 +635,14 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="4">
         <v>69</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -633,10 +652,10 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="1" t="s">
         <v>4</v>
       </c>
@@ -644,10 +663,10 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="1" t="s">
         <v>7</v>
       </c>
@@ -655,14 +674,14 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="4">
         <v>60</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -672,10 +691,10 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="1" t="s">
         <v>22</v>
       </c>
@@ -683,10 +702,10 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="1" t="s">
         <v>4</v>
       </c>
@@ -694,14 +713,14 @@
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="4">
         <v>193</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="4" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -711,10 +730,10 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5"/>
       <c r="F16" s="1" t="s">
         <v>9</v>
       </c>
@@ -722,10 +741,10 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
       <c r="F17" s="1" t="s">
         <v>10</v>
       </c>
@@ -733,6 +752,9 @@
       <c r="H17" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="B21" s="2" t="s">
         <v>12</v>
       </c>
@@ -743,7 +765,13 @@
         <v>16</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -754,12 +782,20 @@
         <v>24</v>
       </c>
       <c r="C22" s="1">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D22" s="1">
         <v>6</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1">
+        <v>44.31</v>
+      </c>
+      <c r="F22" s="1">
+        <v>935.51</v>
+      </c>
+      <c r="G22" s="1">
+        <v>988.67</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
@@ -769,12 +805,20 @@
         <v>27</v>
       </c>
       <c r="C23" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D23" s="1">
         <v>3</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1">
+        <v>26.32</v>
+      </c>
+      <c r="F23" s="1">
+        <v>180.21</v>
+      </c>
+      <c r="G23" s="1">
+        <v>205.1</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
@@ -784,12 +828,20 @@
         <v>25</v>
       </c>
       <c r="C24" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D24" s="1">
         <v>5</v>
       </c>
-      <c r="E24" s="1"/>
+      <c r="E24" s="1">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="F24" s="1">
+        <v>236.66</v>
+      </c>
+      <c r="G24" s="1">
+        <v>245.58</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
@@ -799,12 +851,20 @@
         <v>14</v>
       </c>
       <c r="C25" s="1">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D25" s="1">
         <v>7</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1">
+        <v>67.36</v>
+      </c>
+      <c r="F25" s="1">
+        <v>406.18</v>
+      </c>
+      <c r="G25" s="1">
+        <v>404.73</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
@@ -818,6 +878,8 @@
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -831,6 +893,8 @@
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
@@ -840,23 +904,39 @@
         <v>26</v>
       </c>
       <c r="C28" s="1">
-        <v>109</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+        <v>154</v>
+      </c>
+      <c r="D28" s="1">
+        <v>39</v>
+      </c>
+      <c r="E28" s="1">
+        <v>44.52</v>
+      </c>
+      <c r="F28" s="1">
+        <v>795.5</v>
+      </c>
+      <c r="G28" s="1">
+        <v>735.34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="1">
+        <f>SUM(C22:C28)</f>
+        <v>428</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="5"/>
+      <c r="B33" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="C15:C17"/>
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="E6:E8"/>
     <mergeCell ref="E12:E14"/>
@@ -865,10 +945,17 @@
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D12:D14"/>
     <mergeCell ref="D6:D8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="C15:C17"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
     <mergeCell ref="C12:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
starting on the angelic choice example
</commit_message>
<xml_diff>
--- a/benchmarks/effects/results.xlsx
+++ b/benchmarks/effects/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yahuis/Desktop/git/AlgebraicEffect/benchmarks/effects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4970C29C-930C-BB42-99DA-369DE76936D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0117C6-BB0D-564D-84FE-DFC1ABB9C553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="600" windowWidth="28040" windowHeight="17440" xr2:uid="{F224C7BA-0B0B-E048-B52D-6A1651DC64AD}"/>
   </bookViews>
@@ -134,7 +134,7 @@
     <t>#</t>
   </si>
   <si>
-    <t>Totol</t>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
   <dimension ref="A2:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -927,10 +927,22 @@
         <f>SUM(C22:C28)</f>
         <v>428</v>
       </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="D29" s="1">
+        <f>SUM(D22:D28)</f>
+        <v>60</v>
+      </c>
+      <c r="E29" s="1">
+        <f>SUM(E22:E28)</f>
+        <v>215.21</v>
+      </c>
+      <c r="F29" s="1">
+        <f>SUM(F22:F28)</f>
+        <v>2554.0600000000004</v>
+      </c>
+      <c r="G29" s="1">
+        <f>SUM(G22:G28)</f>
+        <v>2579.42</v>
+      </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="3"/>

</xml_diff>

<commit_message>
writing spec for B
</commit_message>
<xml_diff>
--- a/benchmarks/effects/results.xlsx
+++ b/benchmarks/effects/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yahuis/Desktop/git/AlgebraicEffect/benchmarks/effects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0117C6-BB0D-564D-84FE-DFC1ABB9C553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C1EEBD-8480-D341-9AFB-19134F48BB4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="600" windowWidth="28040" windowHeight="17440" xr2:uid="{F224C7BA-0B0B-E048-B52D-6A1651DC64AD}"/>
   </bookViews>
@@ -520,7 +520,7 @@
   <dimension ref="A2:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
spliting the cases for helper
</commit_message>
<xml_diff>
--- a/benchmarks/effects/results.xlsx
+++ b/benchmarks/effects/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yahuis/Desktop/git/AlgebraicEffect/benchmarks/effects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C1EEBD-8480-D341-9AFB-19134F48BB4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BC192D-50A4-F443-8803-F5EC707C4324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="600" windowWidth="28040" windowHeight="17440" xr2:uid="{F224C7BA-0B0B-E048-B52D-6A1651DC64AD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>McCarthy_Andrej_Bauer</t>
   </si>
@@ -517,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA336E8F-A7D0-AB4A-B959-3554529D4463}">
-  <dimension ref="A2:H33"/>
+  <dimension ref="A2:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -874,78 +874,71 @@
         <v>0</v>
       </c>
       <c r="C26" s="1">
-        <v>83</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="D26" s="1">
+        <v>24</v>
+      </c>
+      <c r="E26" s="1">
+        <v>157.30000000000001</v>
+      </c>
+      <c r="F26" s="1">
+        <v>777.93</v>
+      </c>
+      <c r="G26" s="1">
+        <v>891.71</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C27" s="1">
-        <v>70</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+        <v>154</v>
+      </c>
+      <c r="D27" s="1">
+        <v>39</v>
+      </c>
+      <c r="E27" s="1">
+        <v>44.52</v>
+      </c>
+      <c r="F27" s="1">
+        <v>795.5</v>
+      </c>
+      <c r="G27" s="1">
+        <v>735.34</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>7</v>
-      </c>
       <c r="B28" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C28" s="1">
-        <v>154</v>
+        <f>SUM(C22:C27)</f>
+        <v>354</v>
       </c>
       <c r="D28" s="1">
-        <v>39</v>
+        <f>SUM(D22:D27)</f>
+        <v>84</v>
       </c>
       <c r="E28" s="1">
-        <v>44.52</v>
+        <f>SUM(E22:E27)</f>
+        <v>372.51</v>
       </c>
       <c r="F28" s="1">
-        <v>795.5</v>
+        <f>SUM(F22:F27)</f>
+        <v>3331.9900000000002</v>
       </c>
       <c r="G28" s="1">
-        <v>735.34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="1">
-        <f>SUM(C22:C28)</f>
-        <v>428</v>
-      </c>
-      <c r="D29" s="1">
-        <f>SUM(D22:D28)</f>
-        <v>60</v>
-      </c>
-      <c r="E29" s="1">
-        <f>SUM(E22:E28)</f>
-        <v>215.21</v>
-      </c>
-      <c r="F29" s="1">
-        <f>SUM(F22:F28)</f>
-        <v>2554.0600000000004</v>
-      </c>
-      <c r="G29" s="1">
-        <f>SUM(G22:G28)</f>
-        <v>2579.42</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="3"/>
+        <f>SUM(G22:G27)</f>
+        <v>3471.13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="20">

</xml_diff>